<commit_message>
Updated parameters and methods
</commit_message>
<xml_diff>
--- a/config/parameters.xlsx
+++ b/config/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clemson-my.sharepoint.com/personal/agrawa3_clemson_edu/Documents/Current/_spam_detection/spam_detection/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1630" documentId="11_8B9EB9E23FA7566689F0952CCC2E774EB7C715D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57637219-006E-4DB6-A755-5197DCCC24A8}"/>
+  <xr:revisionPtr revIDLastSave="1761" documentId="11_8B9EB9E23FA7566689F0952CCC2E774EB7C715D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{545B7EEC-028B-42FF-AA66-A6AEAB619ACE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="579" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17835" yWindow="0" windowWidth="33870" windowHeight="20985" tabRatio="579" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filepaths" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="176">
   <si>
     <t>flag_name</t>
   </si>
@@ -72,9 +72,6 @@
     <t>parameters</t>
   </si>
   <si>
-    <t>flag_MultipleIPAttempts</t>
-  </si>
-  <si>
     <t>F_RIDFraudScoreHigh</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>F_MultipleFailedAttempts</t>
-  </si>
-  <si>
-    <t>flag_BurstResponses</t>
   </si>
   <si>
     <t>{"column_name" : "Q_RelevantIDFraudScore",
@@ -115,22 +109,10 @@
     <t>flag_group</t>
   </si>
   <si>
-    <t>FG_QS</t>
-  </si>
-  <si>
-    <t>FG_LP</t>
-  </si>
-  <si>
-    <t>FG_HP</t>
-  </si>
-  <si>
     <t>{"list_of_columns" : ["Q8.2_1"],
 "min_length" : 1,
 "max_length" : "inf",
 "search_strategy" : "column"}</t>
-  </si>
-  <si>
-    <t>flag_ReverseCodedResponse</t>
   </si>
   <si>
     <t>F_ReverseAffect</t>
@@ -148,16 +130,7 @@
 "upper_threshold" : 0.49}</t>
   </si>
   <si>
-    <t>FG_IP</t>
-  </si>
-  <si>
-    <t>FG_LQ</t>
-  </si>
-  <si>
     <t>F_InstructedMatrix</t>
-  </si>
-  <si>
-    <t>flag_CustomCondition</t>
   </si>
   <si>
     <t>F_InstructedSelectAll</t>
@@ -217,22 +190,6 @@
   <si>
     <t>{"column_ip" : "IPAddress",
 "column_success" : "Q7.1", 
-"num_attempts_lower" : 3,
-"num_attempts_upper" : "inf",
-"attempt_type" : "successful",
-"column_terminate" : "Q_TerminateFlag"}</t>
-  </si>
-  <si>
-    <t>{"column_ip" : "IPAddress",
-"column_success" : "Q7.1", 
-"num_attempts_lower" : 2,
-"num_attempts_upper" : 2,
-"attempt_type" : "successful",
-"column_terminate" : null}</t>
-  </si>
-  <si>
-    <t>{"column_ip" : "IPAddress",
-"column_success" : "Q7.1", 
 "num_attempts_lower" : 2,
 "num_attempts_upper" : "inf",
 "attempt_type" : "incomplete",
@@ -242,14 +199,6 @@
     <t>F_MultipleAttempts</t>
   </si>
   <si>
-    <t>{"column_ip" : "IPAddress",
-"column_success" : "Q7.1", 
-"num_attempts_lower" : 2,
-"num_attempts_upper" : "inf",
-"attempt_type" : "all",
-"column_terminate" : "Q_TerminateFlag"}</t>
-  </si>
-  <si>
     <t>{"list_of_columns" : ["Q4.1", "Q7.11", "Q8.1_1", "Q8.1_2"],
 "list_of_chars" : ["\\xa0"]}</t>
   </si>
@@ -265,9 +214,6 @@
 "upper_threshold" : 360}</t>
   </si>
   <si>
-    <t>FG_IN</t>
-  </si>
-  <si>
     <t>F_DuplicateProlificID</t>
   </si>
   <si>
@@ -325,15 +271,9 @@
     <t>Rule 3</t>
   </si>
   <si>
-    <t>(FG_IP &gt; 0) + (FG_QS &gt; 0) + (FG_LP &gt; 0) &gt;= 2</t>
-  </si>
-  <si>
     <t>Rule 4</t>
   </si>
   <si>
-    <t>FG_LQ &gt;= 2</t>
-  </si>
-  <si>
     <t>LOW QUALITY</t>
   </si>
   <si>
@@ -344,9 +284,6 @@
   </si>
   <si>
     <t>VALID</t>
-  </si>
-  <si>
-    <t>(FG_IP &gt; 0) + (FG_QS &gt; 0) + (FG_LP &gt; 0) + (FG_LQ &gt; 0) &gt; 0</t>
   </si>
   <si>
     <t>rule_num</t>
@@ -391,18 +328,6 @@
 "flag_missing" : "false"}</t>
   </si>
   <si>
-    <t>FG_IN &gt; 0</t>
-  </si>
-  <si>
-    <t>FG_HP &gt; 0</t>
-  </si>
-  <si>
-    <t>FG_PD &gt; 0</t>
-  </si>
-  <si>
-    <t>FG_QS &gt;= 2</t>
-  </si>
-  <si>
     <t>use_rule</t>
   </si>
   <si>
@@ -421,16 +346,7 @@
     <t>A hidden question (honeypot) that should not be visible to human respondents. Any response indicates potential automation or bot use.</t>
   </si>
   <si>
-    <t>Verifies if the latitude/longitude data corresponds to the target country. If no location is returned, the response is not flagged unless "flag_missing" is set to "true". A list of valid country names is provided "world-administrative-boundaries-countries.txt".</t>
-  </si>
-  <si>
-    <t>Looks up location using the IP address (using https://ipinfo.io/) and verifies if it matches the target region. If no IP location is found, the response is not flagged unless "flag_missing" is set to "true".</t>
-  </si>
-  <si>
     <t>Identifies identical text responses of ≥31 characters within the same column across different responses. Each column is assessed independently if "search_strategy" is set to "column".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Survey duration is less than 8 minutes, suggesting minimal effort or bot activity, especially when the expected duration is ~15 minutes. </t>
   </si>
   <si>
     <r>
@@ -481,9 +397,6 @@
     </r>
   </si>
   <si>
-    <t>Three or more successful attempts from the same IP subnet (first 3 digits). A same IP subnet indicates a high likelihood of the same Internet network, especially when the time difference in relatively small. A "successful" attempt has a response to a specific question, usually towards the end of the survey.</t>
-  </si>
-  <si>
     <t>Exactly two successful responses from the same IP subnet. A "successful" attempt has a response to a specific question, usually towards the end of the survey.</t>
   </si>
   <si>
@@ -516,15 +429,6 @@
 "column_terminate" : "Q_TerminateFlag"}</t>
   </si>
   <si>
-    <t>Two or more incomplete attempts from the same IP subnet. An "incomplete" attempt has no response to a specific question, usually towards the end of the survey, and has a missing terminate flag.</t>
-  </si>
-  <si>
-    <t>Two or more failed attempts from the same IP subnet. A "failed" attempt has no response to a specific question, usually towards the end of the survey, and has a non-empty terminate flag.</t>
-  </si>
-  <si>
-    <t>Two or more attempts from the same IP subnet, including all types of attempts (successful, incomplete, failed).</t>
-  </si>
-  <si>
     <t xml:space="preserve">Flags responses where the product of the mean normalized scores for positive and negative affect items is ≥ 0.2. Since each item has a single response, the product is used as a proxy for their within-response association; high values may suggest inconsistent affect patterns. </t>
   </si>
   <si>
@@ -643,6 +547,132 @@
   </si>
   <si>
     <t>./data/fuzz_7.11.csv</t>
+  </si>
+  <si>
+    <t>check_ReverseCodedResponse</t>
+  </si>
+  <si>
+    <t>data_used</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>{"column_ip" : "IPAddress",
+"column_success" : "Q7.1", 
+"num_attempts_lower" : 3,
+"num_attempts_upper" : "inf",
+"attempt_type" : "successful"}</t>
+  </si>
+  <si>
+    <t>Verifies if the latitude/longitude data corresponds to the target country. If no location is returned (e.g., lat-long falls within a water body), the response is not flagged unless "flag_missing" is set to "true". A list of valid country names is provided "world-administrative-boundaries-countries.txt".</t>
+  </si>
+  <si>
+    <t>Metadata; Survey question</t>
+  </si>
+  <si>
+    <t>Survey question</t>
+  </si>
+  <si>
+    <t>Qualtrics security feature</t>
+  </si>
+  <si>
+    <t>F_MultipleUnsuccessfulAttempts</t>
+  </si>
+  <si>
+    <t>{"column_ip" : "IPAddress",
+"column_success" : "Q7.1", 
+"num_attempts_lower" : 3,
+"num_attempts_upper" : "inf",
+"attempt_type" : "unsuccessful"}</t>
+  </si>
+  <si>
+    <t>{"column_ip" : "IPAddress",
+"column_success" : "Q7.1", 
+"num_attempts_lower" : 2,
+"num_attempts_upper" : 2,
+"attempt_type" : "successful"}</t>
+  </si>
+  <si>
+    <t>Two or more attempts from the same IP subnet, including both successful and unsuccessful attempts.</t>
+  </si>
+  <si>
+    <t>{"column_ip" : "IPAddress",
+"column_success" : "Q7.1", 
+"num_attempts_lower" : 2,
+"num_attempts_upper" : "inf",
+"attempt_type" : "all"}</t>
+  </si>
+  <si>
+    <t>Three or more unsuccessful attempts from the same IP subnet (first 3 digits). A same IP subnet indicates a high likelihood of the same Internet network, especially when the time difference in relatively small. An attempt is considered "unsuccessful" if "column_success" has an empty response. "column_success" should typically be a question towards the end of the survey.</t>
+  </si>
+  <si>
+    <t>Three or more successful attempts from the same IP subnet (first 3 digits). A same IP subnet indicates a high likelihood of the same Internet network, especially when the time difference in relatively small. An attempt is considered "successful" if "column_success" has a non-empty response. "column_success" should typically be a question towards the end of the survey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two or more failed attempts from the same IP subnet. An attempt is considered "failed" if "column_success" has no response, and has a non-empty terminate flag. "column_success" should typically be a question towards the end of the survey. </t>
+  </si>
+  <si>
+    <t>Two or more incomplete attempts from the same IP subnet. An attempt is considered "incomplete" if "column_success" has no response, and has an empty terminate flag. "column_success" should typically be a question towards the end of the survey.</t>
+  </si>
+  <si>
+    <t>FG_HighPotentialFraud</t>
+  </si>
+  <si>
+    <t>FG_HighPotentialFraud &gt; 0</t>
+  </si>
+  <si>
+    <t>FG_Incomplete</t>
+  </si>
+  <si>
+    <t>FG_Incomplete &gt; 0</t>
+  </si>
+  <si>
+    <t>FG_IPAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Use it only if F_LatLongLocation is unavailable] Looks up location using the IP address (using https://ipinfo.io/) and verifies if it matches the target region. If no IP location is found, the response is not flagged unless "flag_missing" is set to "true". </t>
+  </si>
+  <si>
+    <t>FG_Prolific &gt; 0</t>
+  </si>
+  <si>
+    <t>FG_Prolific</t>
+  </si>
+  <si>
+    <t>FG_LowPotentialFraud</t>
+  </si>
+  <si>
+    <t>FG_QualtricsSecurity &gt;= 2</t>
+  </si>
+  <si>
+    <t>(FG_IPAddress &gt; 0) + (FG_QualtricsSecurity &gt; 0) + (FG_LowPotentialFraud &gt; 0) &gt;= 2</t>
+  </si>
+  <si>
+    <t>FG_QualtricsSecurity</t>
+  </si>
+  <si>
+    <t>FG_LowQuality</t>
+  </si>
+  <si>
+    <t>FG_LowQuality &gt;= 2</t>
+  </si>
+  <si>
+    <t>(FG_IPAddress &gt; 0) + (FG_QualtricsSecurity &gt; 0) + (FG_LowPotentialFraud &gt; 0) + (FG_LowQuality &gt; 0) &gt; 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey duration is less than 6 minutes, suggesting minimal effort or bot activity, especially when the expected duration is ~15 minutes. </t>
+  </si>
+  <si>
+    <t>F_ShortDuration</t>
+  </si>
+  <si>
+    <t>{"column_name" : "Duration (in seconds)",
+"lower_threshold" : 361,
+"upper_threshold" : 480}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey duration is between 6-8 minutes, suggesting minimal effort or potential bot activity, especially when the expected duration is ~15 minutes. </t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1057,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1038,79 +1068,79 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1120,25 +1150,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A7FDCC-5419-4B65-A953-81A295F3903C}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="34" style="3" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39" style="3" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="59.140625" style="3" customWidth="1"/>
     <col min="7" max="16384" width="30.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1146,10 +1176,10 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>9</v>
@@ -1157,486 +1187,634 @@
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="B19" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
+        <v>161</v>
       </c>
       <c r="D19" s="3">
         <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>59</v>
+        <v>148</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>75</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="D20" s="3">
         <v>0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="D21" s="3">
         <v>0</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>10</v>
+        <v>76</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="D22" s="3">
         <v>0</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>10</v>
+        <v>77</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="D23" s="3">
         <v>0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>123</v>
+        <v>28</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>73</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="D25" s="3">
         <v>0</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>16</v>
+        <v>140</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="D26" s="3">
         <v>0</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>130</v>
+      <c r="F28" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{04A7FDCC-5419-4B65-A953-81A295F3903C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F26">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F27">
       <sortCondition descending="1" ref="D1"/>
     </sortState>
   </autoFilter>
@@ -1650,39 +1828,39 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98" style="5" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1690,13 +1868,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1704,13 +1882,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1718,13 +1896,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1732,13 +1910,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1746,13 +1924,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1760,13 +1938,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1774,13 +1952,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1807,27 +1985,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1835,13 +2013,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1849,13 +2027,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1863,13 +2041,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1877,13 +2055,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1891,13 +2069,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1905,13 +2083,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1919,13 +2097,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1946,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFD08D1-5746-4904-A6AE-959AD67C0E82}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,30 +2139,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="E1" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="D2">
         <v>65</v>
@@ -1992,19 +2170,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="D3">
         <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fuzzy string matching details
</commit_message>
<xml_diff>
--- a/config/parameters.xlsx
+++ b/config/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clemson-my.sharepoint.com/personal/agrawa3_clemson_edu/Documents/Current/_spam_detection/spam_detection/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1798" documentId="11_8B9EB9E23FA7566689F0952CCC2E774EB7C715D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7697F63-5656-4D82-8A54-3A4EE9E57DCF}"/>
+  <xr:revisionPtr revIDLastSave="1800" documentId="11_8B9EB9E23FA7566689F0952CCC2E774EB7C715D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E87B402-939A-4540-8B71-795B4C51DFAF}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="579" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53265" yWindow="2580" windowWidth="28905" windowHeight="17865" tabRatio="579" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filepaths" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="174">
   <si>
     <t>flag_name</t>
   </si>
@@ -541,12 +541,6 @@
   </si>
   <si>
     <t>File path to create optional file that contains information on similar text responses. Requires inputs in the "fuzzy_string" sheet.</t>
-  </si>
-  <si>
-    <t>maxtrix_filepath</t>
-  </si>
-  <si>
-    <t>./data/fuzz_7.11.csv</t>
   </si>
   <si>
     <t>check_ReverseCodedResponse</t>
@@ -1044,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225C0359-8BE7-4634-82D1-A1988AB19DA9}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1196,7 +1190,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -1208,10 +1202,10 @@
         <v>81</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1219,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1234,7 +1228,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1242,7 +1236,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1251,13 +1245,13 @@
         <v>75</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1265,7 +1259,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -1280,7 +1274,7 @@
         <v>89</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1288,7 +1282,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1300,10 +1294,10 @@
         <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1311,7 +1305,7 @@
         <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1326,7 +1320,7 @@
         <v>90</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1334,7 +1328,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1343,13 +1337,13 @@
         <v>75</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>91</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1357,7 +1351,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -1372,7 +1366,7 @@
         <v>92</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1380,7 +1374,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1395,7 +1389,7 @@
         <v>94</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1403,7 +1397,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -1418,7 +1412,7 @@
         <v>95</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1426,7 +1420,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -1441,7 +1435,7 @@
         <v>97</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1449,7 +1443,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -1464,7 +1458,7 @@
         <v>98</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1472,7 +1466,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -1487,7 +1481,7 @@
         <v>87</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1495,7 +1489,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -1507,10 +1501,10 @@
         <v>79</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1518,7 +1512,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1533,7 +1527,7 @@
         <v>86</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1541,7 +1535,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -1553,10 +1547,10 @@
         <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1564,7 +1558,7 @@
         <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -1573,13 +1567,13 @@
         <v>75</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1587,7 +1581,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1599,18 +1593,18 @@
         <v>99</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -1619,13 +1613,13 @@
         <v>75</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1633,7 +1627,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -1648,15 +1642,15 @@
         <v>93</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -1665,13 +1659,13 @@
         <v>76</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1679,7 +1673,7 @@
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -1694,7 +1688,7 @@
         <v>103</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1702,7 +1696,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -1717,7 +1711,7 @@
         <v>96</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1725,7 +1719,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -1740,7 +1734,7 @@
         <v>104</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -1748,13 +1742,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>22</v>
@@ -1763,7 +1757,7 @@
         <v>100</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1771,7 +1765,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -1786,7 +1780,7 @@
         <v>101</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1794,7 +1788,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -1809,7 +1803,7 @@
         <v>102</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1853,7 +1847,7 @@
         <v>61</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -1867,7 +1861,7 @@
         <v>113</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
         <v>62</v>
@@ -1881,7 +1875,7 @@
         <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
@@ -1895,7 +1889,7 @@
         <v>119</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
         <v>62</v>
@@ -1909,7 +1903,7 @@
         <v>120</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
         <v>62</v>
@@ -1923,7 +1917,7 @@
         <v>64</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
         <v>66</v>
@@ -1937,7 +1931,7 @@
         <v>65</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
         <v>68</v>
@@ -2118,67 +2112,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFD08D1-5746-4904-A6AE-959AD67C0E82}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>128</v>
       </c>
       <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
       <c r="B2">
+        <v>65</v>
+      </c>
+      <c r="C2">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>134</v>
       </c>
-      <c r="D2">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>133</v>
       </c>
       <c r="B3">
+        <v>65</v>
+      </c>
+      <c r="C3">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>134</v>
-      </c>
-      <c r="D3">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor updates to docs
</commit_message>
<xml_diff>
--- a/config/parameters.xlsx
+++ b/config/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clemson-my.sharepoint.com/personal/agrawa3_clemson_edu/Documents/Current/_spam_detection/spam_detection/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1800" documentId="11_8B9EB9E23FA7566689F0952CCC2E774EB7C715D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E87B402-939A-4540-8B71-795B4C51DFAF}"/>
+  <xr:revisionPtr revIDLastSave="1806" documentId="11_8B9EB9E23FA7566689F0952CCC2E774EB7C715D3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D978901-274E-4AD9-A140-5BF2908CDB74}"/>
   <bookViews>
-    <workbookView xWindow="53265" yWindow="2580" windowWidth="28905" windowHeight="17865" tabRatio="579" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="579" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="filepaths" sheetId="6" r:id="rId1"/>
@@ -247,9 +247,6 @@
     <t>./figures/</t>
   </si>
   <si>
-    <t>./data/sample_data.csv</t>
-  </si>
-  <si>
     <t>condition_expr</t>
   </si>
   <si>
@@ -525,12 +522,6 @@
     <t>threshold</t>
   </si>
   <si>
-    <t>Q4.1</t>
-  </si>
-  <si>
-    <t>Q7.11</t>
-  </si>
-  <si>
     <t>token_sort_ratio</t>
   </si>
   <si>
@@ -667,6 +658,15 @@
   </si>
   <si>
     <t xml:space="preserve">Survey duration is between 6-8 minutes, suggesting minimal effort or potential bot activity, especially when the expected duration is ~15 minutes. </t>
+  </si>
+  <si>
+    <t>./data/sample_data.csv</t>
+  </si>
+  <si>
+    <t>Q4.1</t>
+  </si>
+  <si>
+    <t>Q7.11</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225C0359-8BE7-4634-82D1-A1988AB19DA9}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1065,7 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1087,10 +1087,10 @@
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,40 +1101,40 @@
         <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
         <v>123</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>124</v>
-      </c>
-      <c r="C7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1182,30 +1182,30 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1213,22 +1213,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1236,22 +1236,22 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1259,22 +1259,22 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1282,22 +1282,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1305,22 +1305,22 @@
         <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1328,22 +1328,22 @@
         <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1351,22 +1351,22 @@
         <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1374,22 +1374,22 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1397,22 +1397,22 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1420,22 +1420,22 @@
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1443,22 +1443,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1466,22 +1466,22 @@
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1489,22 +1489,22 @@
         <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1512,22 +1512,22 @@
         <v>17</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1535,22 +1535,22 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1558,22 +1558,22 @@
         <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1581,45 +1581,45 @@
         <v>14</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1627,45 +1627,45 @@
         <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1673,22 +1673,22 @@
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1696,22 +1696,22 @@
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1719,22 +1719,22 @@
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -1742,22 +1742,22 @@
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1765,22 +1765,22 @@
         <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1788,22 +1788,22 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1830,27 +1830,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1858,13 +1858,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1886,13 +1886,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1900,13 +1900,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1914,13 +1914,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1928,13 +1928,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1942,13 +1942,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1975,27 +1975,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2003,13 +2003,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2017,13 +2017,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2031,13 +2031,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2045,13 +2045,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
         <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>107</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2059,13 +2059,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2073,13 +2073,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2087,13 +2087,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2114,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFD08D1-5746-4904-A6AE-959AD67C0E82}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,21 +2128,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>129</v>
-      </c>
-      <c r="D1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B2">
         <v>65</v>
@@ -2151,12 +2151,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>65</v>
@@ -2165,7 +2165,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>